<commit_message>
refactor: unify heat and gas hydraulic calculation
</commit_message>
<xml_diff>
--- a/SolUtil/energyflow/test/test_dhs_flow/BarryIsland.xlsx
+++ b/SolUtil/energyflow/test/test_dhs_flow/BarryIsland.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="53" documentId="114_{77C003BD-D8EC-4B1D-A3A4-E18C67D8E4B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5C8D9449-F41B-4B51-863D-D54CEBFEC61F}"/>
+  <xr:revisionPtr revIDLastSave="59" documentId="114_{77C003BD-D8EC-4B1D-A3A4-E18C67D8E4B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9AE3D5BF-B9C2-46EC-8F35-E35676D0E64A}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="772" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3000,7 +3000,7 @@
   <dimension ref="A1:A36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3012,7 +3012,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>9.6189160000000005</v>
+        <v>9.6189149999999994</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
@@ -3027,7 +3027,7 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>-5.0540000000000002E-2</v>
+        <v>-5.0541000000000003E-2</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
@@ -3037,12 +3037,12 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>-23.491288999999998</v>
+        <v>-23.491289999999999</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>5.5211389999999998</v>
+        <v>5.5211379999999997</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
@@ -3052,7 +3052,7 @@
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>3.0647579999999999</v>
+        <v>3.0647570000000002</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
@@ -3072,7 +3072,7 @@
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>7.8614699999999997</v>
+        <v>7.8614689999999996</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
@@ -3112,7 +3112,7 @@
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>-1.8389450000000001</v>
+        <v>-1.838946</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
@@ -3172,7 +3172,7 @@
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>19.16638</v>
+        <v>19.166381000000001</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
@@ -3196,7 +3196,7 @@
   <dimension ref="A1:A36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A2" sqref="A2:A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3392,7 +3392,7 @@
   <dimension ref="A1:A36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J36" sqref="J36"/>
+      <selection activeCell="A2" sqref="A2:A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3587,7 +3587,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA8A46AB-BC61-47EC-BC5E-CA1F25AC8FBF}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>

</xml_diff>